<commit_message>
Updated Dashboard with 10th grade ELA content layout.
To-Do: Write functions to calculate available points for Fiction/Non-Fiction and Num Texts
</commit_message>
<xml_diff>
--- a/data/2022MCASItemXWalk.xlsx
+++ b/data/2022MCASItemXWalk.xlsx
@@ -118,7 +118,7 @@
     <t>W.PK-12.1 W.PK-12.4</t>
   </si>
   <si>
-    <t>Idea Develoment</t>
+    <t>Idea Development</t>
   </si>
   <si>
     <t>Argumentative and Structure</t>
@@ -22919,7 +22919,7 @@
       <c r="A17" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="22" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="25" t="s">
@@ -22930,7 +22930,7 @@
       <c r="A18" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="22" t="s">
         <v>32</v>
       </c>
       <c r="C18" s="25" t="s">
@@ -26838,14 +26838,14 @@
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B19:B22">
-      <formula1>"Conventions,Craft and Structure,Key Ideas and Details,Vocabulary Acquisition and Use,Idea Develoment,Integration of Knowledge and Ideas,WR Combined (Conv/Idea Dev),Knowledge of Language,Text Types and Purposes"</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B18">
+      <formula1>"Conventions,Craft and Structure,Key Ideas and Details,Vocabulary Acquisition and Use,Idea Development,Integration of Knowledge and Ideas,WR Combined (Conv/Idea Dev),Knowledge of Language"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B23">
       <formula1>"Conventions,Craft and Structure,Key Ideas and Details,Vocabulary Acquisition and Use,Idea Develoment,Integration of Knowledge and Ideas,WR Combined (Conv/Idea Dev),Knowledge of Language,Text Types and Purposes,Production and Distribution of Writing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B18">
-      <formula1>"Conventions,Craft and Structure,Key Ideas and Details,Vocabulary Acquisition and Use,Idea Develoment,Integration of Knowledge and Ideas,WR Combined (Conv/Idea Dev),Knowledge of Language"</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B19:B22">
+      <formula1>"Conventions,Craft and Structure,Key Ideas and Details,Vocabulary Acquisition and Use,Idea Development,Integration of Knowledge and Ideas,WR Combined (Conv/Idea Dev),Knowledge of Language,Text Types and Purposes"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>

</xml_diff>

<commit_message>
Updated Student Performance Function Library Need to debug the Practice Category Function with ELA10 tests
</commit_message>
<xml_diff>
--- a/data/2022MCASItemXWalk.xlsx
+++ b/data/2022MCASItemXWalk.xlsx
@@ -8,11 +8,11 @@
     <sheet state="visible" name="SG8_practice_xwalk" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="SG5_practice_xwalk" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="ELA_cluster_xwalk" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="ELA10_xwalk" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="ELA8_xwalk" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="ELA7_xwalk" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="ELA6_xwalk" sheetId="9" r:id="rId12"/>
-    <sheet state="visible" name="ELA5_xwalk" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="EG10_xwalk" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="EG8_xwalk" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="EG7_xwalk" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="EG6_xwalk" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="EG5_xwalk" sheetId="10" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="125">
   <si>
     <t>ITEM</t>
   </si>
@@ -232,6 +232,42 @@
     <t>WR9.IDEA1</t>
   </si>
   <si>
+    <t>Starfish, Akemi Dawn Bowman</t>
+  </si>
+  <si>
+    <t>The Poet X, Elizabeth Aceva: Novel in Verse</t>
+  </si>
+  <si>
+    <t>Both fiction texts: Starfish, The Poet X read in previous 7 items</t>
+  </si>
+  <si>
+    <t>Write Essay and Cite evidence from: Both fiction texts: Starfish, The Poet X read in previous 7 items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Man Who Went to the Far Side of the Moon, Biography: </t>
+  </si>
+  <si>
+    <t>"First Men on the Moon", Poem about the Moon Landing</t>
+  </si>
+  <si>
+    <t>Both Non-fiction texts: "The Man Who Went to the Far Side of the Moon", "First Men on the Moon" read in previous 5 items</t>
+  </si>
+  <si>
+    <t>Unreleased: item description references an excerpt</t>
+  </si>
+  <si>
+    <t>Unreleased: item description references a passage</t>
+  </si>
+  <si>
+    <t>Unreleased: item description references a passage and a character</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>Unreleased: Item description references an excerpt and passage on same topic</t>
+  </si>
+  <si>
     <t>LA12.CONV1</t>
   </si>
   <si>
@@ -244,6 +280,48 @@
     <t>WR31.IDEA2</t>
   </si>
   <si>
+    <t>Article, "The Teen Who Woke up her School", Jane Bianchi</t>
+  </si>
+  <si>
+    <t>Article, 'Why Schools are Struggling to Let Students Sleep In"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both Non-fiction articles "The Teen Who Woke up her School" and "Why Schools are Struggling to Let Students Sleep in" in previous 10 questions </t>
+  </si>
+  <si>
+    <t>Play, adaptation of "The Emperors New Clothes"</t>
+  </si>
+  <si>
+    <t>? Unreleased Item description references character's point of view in passage</t>
+  </si>
+  <si>
+    <t>? Unreleased Item description references idea of a passage</t>
+  </si>
+  <si>
+    <t>? Unreleased Item description references mood of a passage</t>
+  </si>
+  <si>
+    <t>? Unreleased Item description references significance of a passage</t>
+  </si>
+  <si>
+    <t>? Unreleased Item description references central idea of a passage</t>
+  </si>
+  <si>
+    <t>? Unreleased Item description references determining meaning of a word in context</t>
+  </si>
+  <si>
+    <t>? Unreleased Item description references making an inference from a passage</t>
+  </si>
+  <si>
+    <t>? Unreleaded item descripton references analyzing how paragraphs in a passage impact characterization.</t>
+  </si>
+  <si>
+    <t>? Unreleased, item description references 2 authors</t>
+  </si>
+  <si>
+    <t>? Unreleased, references 2 different passages</t>
+  </si>
+  <si>
     <t>WR13.IDEA1</t>
   </si>
   <si>
@@ -254,6 +332,69 @@
   </si>
   <si>
     <t>LA32.CONV2</t>
+  </si>
+  <si>
+    <t>Ways to Reuse Items to Save Money and Reduce Waste, Amy Livingston</t>
+  </si>
+  <si>
+    <t>The Junction of Sunshine and Lucky, Holly Schindler</t>
+  </si>
+  <si>
+    <t>Prior Non-Fiction Article and Fiction Passage in 1-8 tems</t>
+  </si>
+  <si>
+    <t>The Secret of the Rat Cat, Sharon Pochran</t>
+  </si>
+  <si>
+    <t>?Unreleased, description references a passage</t>
+  </si>
+  <si>
+    <t>?Unreleased, description references a sentence</t>
+  </si>
+  <si>
+    <t>?Unreleased, description references a passage with figurative language</t>
+  </si>
+  <si>
+    <t>?Unreleased, description references tone of a passage</t>
+  </si>
+  <si>
+    <t>?Unreleased, description references a character's point of view</t>
+  </si>
+  <si>
+    <t>?Unreleased, description references word choice in a passage</t>
+  </si>
+  <si>
+    <t>?Unreleased, description references character in a passage</t>
+  </si>
+  <si>
+    <t>?Unreleased, description references the theme in a passage</t>
+  </si>
+  <si>
+    <t>Prompt references explaining methods an author uses to make a passage interesting</t>
+  </si>
+  <si>
+    <t>Saving Marty, Paul Griffin</t>
+  </si>
+  <si>
+    <t>Based on the text read in previous 11 items, write a narrative</t>
+  </si>
+  <si>
+    <t>Keiko Narhashi, "Talking with Artistis"</t>
+  </si>
+  <si>
+    <t>Unreleased, references 1 passage</t>
+  </si>
+  <si>
+    <t>Unreleased, references 1 article</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unreleased, references 1 article and summarry, so seems to be the later progression of an article analyzed </t>
+  </si>
+  <si>
+    <t>Unreleased, says to compare information from an article and a passage on similar topics (Most likely the two readings from earlier in the test)</t>
+  </si>
+  <si>
+    <t>Unreleased but write an essay explaining the feelings of an individual in an article and a passage</t>
   </si>
 </sst>
 </file>
@@ -406,7 +547,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -514,6 +655,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4991,7 +5135,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
@@ -5013,246 +5160,481 @@
       <c r="A2" s="12">
         <v>1.0</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="13">
         <v>2.0</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="6"/>
+      <c r="B3" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="12">
         <v>3.0</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="6"/>
+      <c r="B4" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="13">
         <v>4.0</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="6"/>
+      <c r="B5" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="12">
         <v>5.0</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
+      <c r="B6" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="13">
         <v>6.0</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
+      <c r="B7" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="12">
         <v>7.0</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
+      <c r="B8" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="13">
         <v>8.0</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+      <c r="B9" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="12">
         <v>9.0</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
+      <c r="B10" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="13">
         <v>10.0</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="12">
         <v>11.0</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="6"/>
+      <c r="B12" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="13">
         <v>12.0</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="B13" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="12">
         <v>13.0</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
+      <c r="B14" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="13">
         <v>14.0</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="6"/>
+      <c r="B15" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="12">
         <v>15.0</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="6"/>
+      <c r="B16" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="13">
         <v>16.0</v>
       </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="6"/>
+      <c r="B17" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="12">
         <v>17.0</v>
       </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="6"/>
+      <c r="B18" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="13">
         <v>18.0</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
+      <c r="B19" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="12">
         <v>19.0</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
+      <c r="B20" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="13">
         <v>20.0</v>
       </c>
-      <c r="B21" s="6"/>
+      <c r="B21" s="4">
+        <v>1.0</v>
+      </c>
       <c r="C21" s="6"/>
+      <c r="D21" s="25" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="12">
         <v>21.0</v>
       </c>
-      <c r="B22" s="6"/>
+      <c r="B22" s="4">
+        <v>1.0</v>
+      </c>
       <c r="C22" s="6"/>
+      <c r="D22" s="25" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="13">
         <v>22.0</v>
       </c>
-      <c r="B23" s="6"/>
+      <c r="B23" s="4">
+        <v>1.0</v>
+      </c>
       <c r="C23" s="6"/>
+      <c r="D23" s="25" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="12">
         <v>23.0</v>
       </c>
-      <c r="B24" s="30"/>
+      <c r="B24" s="36">
+        <v>1.0</v>
+      </c>
       <c r="C24" s="6"/>
+      <c r="D24" s="25" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="13">
         <v>24.0</v>
       </c>
-      <c r="B25" s="30"/>
-      <c r="C25" s="6"/>
+      <c r="B25" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="12">
         <v>25.0</v>
       </c>
-      <c r="B26" s="30"/>
+      <c r="B26" s="36">
+        <v>1.0</v>
+      </c>
       <c r="C26" s="6"/>
+      <c r="D26" s="25" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="13">
         <v>26.0</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="6"/>
+      <c r="B27" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="12">
         <v>27.0</v>
       </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="6"/>
+      <c r="B28" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="13">
         <v>28.0</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
+      <c r="B29" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="12">
         <v>29.0</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
+      <c r="B30" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="13">
         <v>30.0</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
+      <c r="B31" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="12">
         <v>31.0</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
+      <c r="B32" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
+        <v>84</v>
+      </c>
+      <c r="B33" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="25" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
+        <v>82</v>
+      </c>
+      <c r="B34" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
+        <v>85</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
+        <v>83</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="6"/>
@@ -22754,9 +23136,15 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="25.13"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
@@ -26882,7 +27270,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
@@ -33224,7 +33615,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
@@ -33268,246 +33662,477 @@
       <c r="A2" s="12">
         <v>1.0</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="13">
         <v>2.0</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="6"/>
+      <c r="B3" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="12">
         <v>3.0</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="6"/>
+      <c r="B4" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="13">
         <v>4.0</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="6"/>
+      <c r="B5" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="12">
         <v>5.0</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
+      <c r="B6" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="13">
         <v>6.0</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
+      <c r="B7" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="12">
         <v>7.0</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
+      <c r="B8" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="13">
         <v>8.0</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+      <c r="B9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="12">
         <v>9.0</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
+      <c r="B10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="13">
         <v>10.0</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="12">
         <v>11.0</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="6"/>
+      <c r="B12" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="13">
         <v>12.0</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="B13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="12">
         <v>13.0</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
+      <c r="B14" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="13">
         <v>14.0</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="6"/>
+      <c r="B15" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="12">
         <v>15.0</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="6"/>
+      <c r="B16" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="13">
         <v>16.0</v>
       </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="6"/>
+      <c r="B17" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="12">
         <v>17.0</v>
       </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="6"/>
+      <c r="B18" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="13">
         <v>18.0</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
+      <c r="B19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="12">
         <v>19.0</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
+      <c r="B20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="13">
         <v>20.0</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
+      <c r="B21" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="25" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="12">
         <v>21.0</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
+      <c r="B22" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="25" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="13">
         <v>22.0</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
+      <c r="B23" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="25" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="12">
         <v>23.0</v>
       </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="6"/>
+      <c r="B24" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="25" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="13">
         <v>24.0</v>
       </c>
-      <c r="B25" s="30"/>
-      <c r="C25" s="6"/>
+      <c r="B25" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="25" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="12">
         <v>25.0</v>
       </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="6"/>
+      <c r="B26" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="25" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="13">
         <v>26.0</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="6"/>
+      <c r="B27" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="25" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="12">
         <v>27.0</v>
       </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="6"/>
+      <c r="B28" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="13">
         <v>28.0</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
+      <c r="B29" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="12">
         <v>29.0</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
+      <c r="B30" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="13">
         <v>30.0</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
+      <c r="B31" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="12">
         <v>31.0</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
+      <c r="B32" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
+        <v>82</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="25" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
+        <v>83</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
+        <v>84</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
+        <v>85</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="6"/>
@@ -38385,7 +39010,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
@@ -38407,253 +39035,493 @@
       <c r="A2" s="3">
         <v>1.0</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="5">
         <v>2.0</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="6"/>
+      <c r="B3" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3">
         <v>3.0</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="6"/>
+      <c r="B4" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="5">
         <v>4.0</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="6"/>
+      <c r="B5" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="3">
         <v>5.0</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
+      <c r="B6" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="5">
         <v>6.0</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
+      <c r="B7" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="3">
         <v>7.0</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
+      <c r="B8" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="5">
         <v>8.0</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+      <c r="B9" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="3">
         <v>9.0</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
+      <c r="B10" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="5">
         <v>10.0</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="3">
         <v>11.0</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="6"/>
+      <c r="B12" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="5">
         <v>12.0</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="B13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="3">
         <v>13.0</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
+      <c r="B14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="5">
         <v>14.0</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="6"/>
+      <c r="B15" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="3">
         <v>15.0</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="6"/>
+      <c r="B16" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="5">
         <v>16.0</v>
       </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="6"/>
+      <c r="B17" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="3">
         <v>17.0</v>
       </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="6"/>
+      <c r="B18" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="5">
         <v>18.0</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
+      <c r="B19" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="3">
         <v>19.0</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
+      <c r="B20" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="5">
         <v>20.0</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
+      <c r="B21" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="3">
         <v>21.0</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
+      <c r="B22" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="5">
         <v>22.0</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
+      <c r="B23" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="3">
         <v>23.0</v>
       </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="6"/>
+      <c r="B24" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="5">
         <v>24.0</v>
       </c>
-      <c r="B25" s="30"/>
-      <c r="C25" s="6"/>
+      <c r="B25" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="3">
         <v>25.0</v>
       </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="6"/>
+      <c r="B26" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="5">
         <v>26.0</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="6"/>
+      <c r="B27" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="3">
         <v>27.0</v>
       </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="6"/>
+      <c r="B28" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="5">
         <v>28.0</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
+      <c r="B29" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="3">
         <v>29.0</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
+      <c r="B30" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="5">
         <v>30.0</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
+      <c r="B31" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="3">
         <v>31.0</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
+      <c r="B32" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="5">
         <v>32.0</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
+      <c r="B33" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="25" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
+        <v>100</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
+        <v>101</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
+        <v>102</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
+        <v>103</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="8"/>
@@ -43527,7 +44395,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
@@ -43549,246 +44420,473 @@
       <c r="A2" s="3">
         <v>1.0</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="5">
         <v>2.0</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="6"/>
+      <c r="B3" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3">
         <v>3.0</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="6"/>
+      <c r="B4" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="5">
         <v>4.0</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="6"/>
+      <c r="B5" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="3">
         <v>5.0</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
+      <c r="B6" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="5">
         <v>6.0</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
+      <c r="B7" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="3">
         <v>7.0</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
+      <c r="B8" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="5">
         <v>8.0</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+      <c r="B9" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="3">
         <v>9.0</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
+      <c r="B10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="5">
         <v>10.0</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="3">
         <v>11.0</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="6"/>
+      <c r="B12" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="5">
         <v>12.0</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="B13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="3">
         <v>13.0</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
+      <c r="B14" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="5">
         <v>14.0</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="6"/>
+      <c r="B15" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="3">
         <v>15.0</v>
       </c>
-      <c r="B16" s="30"/>
-      <c r="C16" s="6"/>
+      <c r="B16" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="5">
         <v>16.0</v>
       </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="6"/>
+      <c r="B17" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="3">
         <v>17.0</v>
       </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="6"/>
+      <c r="B18" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="5">
         <v>18.0</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
+      <c r="B19" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="3">
         <v>19.0</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
+      <c r="B20" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="5">
         <v>20.0</v>
       </c>
-      <c r="B21" s="6"/>
+      <c r="B21" s="4">
+        <v>1.0</v>
+      </c>
       <c r="C21" s="6"/>
+      <c r="D21" s="25" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="3">
         <v>21.0</v>
       </c>
-      <c r="B22" s="6"/>
+      <c r="B22" s="4">
+        <v>1.0</v>
+      </c>
       <c r="C22" s="6"/>
+      <c r="D22" s="25" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="5">
         <v>22.0</v>
       </c>
-      <c r="B23" s="6"/>
+      <c r="B23" s="4">
+        <v>1.0</v>
+      </c>
       <c r="C23" s="6"/>
+      <c r="D23" s="25" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="3">
         <v>23.0</v>
       </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="6"/>
+      <c r="B24" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="5">
         <v>24.0</v>
       </c>
-      <c r="B25" s="30"/>
-      <c r="C25" s="6"/>
+      <c r="B25" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="3">
         <v>25.0</v>
       </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="6"/>
+      <c r="B26" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="5">
         <v>26.0</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="6"/>
+      <c r="B27" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="3">
         <v>27.0</v>
       </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="6"/>
+      <c r="B28" s="36">
+        <v>1.0</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="5">
         <v>28.0</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
+      <c r="B29" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="3">
         <v>29.0</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
+      <c r="B30" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="5">
         <v>30.0</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
+      <c r="B31" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="3">
         <v>31.0</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
+      <c r="B32" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
+        <v>84</v>
+      </c>
+      <c r="B33" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
+        <v>82</v>
+      </c>
+      <c r="B34" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
+        <v>85</v>
+      </c>
+      <c r="B35" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
+        <v>83</v>
+      </c>
+      <c r="B36" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="8"/>

</xml_diff>